<commit_message>
feat: Add dashboard, associate, and leader management pages with associate filtering, status updates, and leader promotion.
</commit_message>
<xml_diff>
--- a/DOCS/PUESTOS DE VOTACION.xlsx
+++ b/DOCS/PUESTOS DE VOTACION.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\repositorio crm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\repositorio crm\connect-people\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A669FA-4CEB-4593-A120-BB530AC78563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBA7407-EEF9-4AE1-BFD2-440F41F4C119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3CBAEA68-EBAF-460C-A328-DF7818CDBF29}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{3CBAEA68-EBAF-460C-A328-DF7818CDBF29}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4814" uniqueCount="2347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4940" uniqueCount="2348">
   <si>
     <t>I.E. SIMON BOLIVAR</t>
   </si>
@@ -7081,6 +7081,9 @@
   </si>
   <si>
     <t>DEPARTAMENTO</t>
+  </si>
+  <si>
+    <t>NO SE</t>
   </si>
 </sst>
 </file>
@@ -7455,8 +7458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FBD94D8-677F-4F94-8DBE-4BADBD620349}">
   <dimension ref="A1:F1203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31537,12 +31540,648 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC4FCD5-1A04-438C-A620-67BEC43AE951}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A126"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection sqref="A1:A126"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1491</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>